<commit_message>
Integrated the config file with the orchestrator assets
</commit_message>
<xml_diff>
--- a/Configuration/Config.xlsx
+++ b/Configuration/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anupam.triwedi\Desktop\Orchestration Template\vb\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\UiPath\OrchestrationProcess\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892AD107-98C7-468D-AB31-81D72C1855DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153A1A0B-C96E-4892-AD23-0F9AEB093A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -41,12 +41,36 @@
   <si>
     <t>OrchestratorAssetFolder</t>
   </si>
+  <si>
+    <t>DocStoragePath</t>
+  </si>
+  <si>
+    <t>InvoiceTrainingData</t>
+  </si>
+  <si>
+    <t>OutputDataFolderPath</t>
+  </si>
+  <si>
+    <t>PurchaseOrderTrainingData</t>
+  </si>
+  <si>
+    <t>Folder path to the documents of the project</t>
+  </si>
+  <si>
+    <t>Folder path the invoice training data</t>
+  </si>
+  <si>
+    <t>Folder path to the output folder</t>
+  </si>
+  <si>
+    <t>Folder path to the purchase order training data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -70,6 +94,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,16 +121,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,15 +449,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -464,15 +495,49 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.5">
-      <c r="C4" s="4"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1480,12 +1545,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1522,7 +1587,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.5">
+    <row r="2" spans="1:26">
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2524,12 +2589,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>